<commit_message>
saida do voiter do conglomerado master
</commit_message>
<xml_diff>
--- a/CODIGO_EMISSOR.xlsx
+++ b/CODIGO_EMISSOR.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\Desktop\categorizador-assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F2B038-5C39-44A3-83E1-2334A89FB89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3C83E7-3A7A-4D5E-B073-8DD86C943B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20745" yWindow="2850" windowWidth="16530" windowHeight="10725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27945" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$150</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$151</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="160">
   <si>
     <t>EMISSOR</t>
   </si>
@@ -500,6 +500,9 @@
   </si>
   <si>
     <t>OURIBANK S.A. BANCO MÚLTIPLO</t>
+  </si>
+  <si>
+    <t>BANCO PLENO S.A. (VOITER)</t>
   </si>
 </sst>
 </file>
@@ -894,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L151"/>
+  <dimension ref="A1:L152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="A152" sqref="A152"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B148" sqref="B148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,8 +2607,19 @@
         <v>7</v>
       </c>
     </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B152" s="5">
+        <v>150</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C150" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C151" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajuste 151 e class
</commit_message>
<xml_diff>
--- a/CODIGO_EMISSOR.xlsx
+++ b/CODIGO_EMISSOR.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\Desktop\categorizador-assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB483C8F-A915-407F-8E36-2EB4495B3501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCB4439-1063-4E92-B90D-F3D779F8130D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27945" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$151</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -262,6 +259,9 @@
     <t>BANCO VOLKSWAGEN</t>
   </si>
   <si>
+    <t>BANCO BV</t>
+  </si>
+  <si>
     <t>BANCO XCMG BRASIL</t>
   </si>
   <si>
@@ -481,35 +481,32 @@
     <t xml:space="preserve">S4 </t>
   </si>
   <si>
+    <t>CONGLOMERADO: MASTER, WILL E LETSBANK</t>
+  </si>
+  <si>
+    <t>NEON/BIORC SCFI</t>
+  </si>
+  <si>
+    <t>OMNI BANCO/OMNI SCFI</t>
+  </si>
+  <si>
+    <t>PARANÁ BANCO S.A.</t>
+  </si>
+  <si>
+    <t>OURIBANK S.A. BANCO MÚLTIPLO</t>
+  </si>
+  <si>
+    <t>BANCO PLENO S.A. (VOITER)</t>
+  </si>
+  <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>BANCO BV</t>
-  </si>
-  <si>
-    <t>NEON/BIORC SCFI</t>
-  </si>
-  <si>
-    <t>OMNI BANCO/OMNI SCFI</t>
-  </si>
-  <si>
-    <t>PARANÁ BANCO S.A.</t>
-  </si>
-  <si>
-    <t>OURIBANK S.A. BANCO MÚLTIPLO</t>
-  </si>
-  <si>
-    <t>BANCO PLENO S.A. (VOITER)</t>
-  </si>
-  <si>
-    <t>CONGLOMERADO: MASTER, WILL E LETSBANK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,29 +520,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -568,33 +552,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFA9D08E"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFA9D08E"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,23 +863,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L152"/>
+  <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -924,7 +887,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -935,7 +898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -946,7 +909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -957,7 +920,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -968,7 +931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -979,7 +942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -990,7 +953,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1001,7 +964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1012,7 +975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1023,7 +986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1034,7 +997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1045,7 +1008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1055,11 +1018,8 @@
       <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1069,11 +1029,8 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1083,11 +1040,8 @@
       <c r="C15" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1097,11 +1051,8 @@
       <c r="C16" t="s">
         <v>9</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1111,11 +1062,8 @@
       <c r="C17" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1125,11 +1073,8 @@
       <c r="C18" t="s">
         <v>9</v>
       </c>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1139,11 +1084,8 @@
       <c r="C19" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1153,11 +1095,8 @@
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1167,11 +1106,8 @@
       <c r="C21" t="s">
         <v>7</v>
       </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1181,11 +1117,8 @@
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1195,11 +1128,8 @@
       <c r="C23" t="s">
         <v>29</v>
       </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1210,7 +1140,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1221,7 +1151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1232,7 +1162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1243,7 +1173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1254,7 +1184,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1265,7 +1195,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1276,7 +1206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1287,7 +1217,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1365,13 +1295,13 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39">
         <v>38</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1409,13 +1339,13 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43">
         <v>42</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1431,13 +1361,13 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45">
         <v>44</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1740,7 +1670,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>153</v>
+        <v>79</v>
       </c>
       <c r="B73">
         <v>72</v>
@@ -1751,7 +1681,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B74">
         <v>73</v>
@@ -1762,7 +1692,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B75">
         <v>74</v>
@@ -1773,7 +1703,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B76">
         <v>75</v>
@@ -1784,7 +1714,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B77">
         <v>76</v>
@@ -1795,7 +1725,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B78">
         <v>77</v>
@@ -1806,7 +1736,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B79">
         <v>78</v>
@@ -1817,7 +1747,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B80">
         <v>79</v>
@@ -1828,7 +1758,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B81">
         <v>80</v>
@@ -1839,7 +1769,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B82">
         <v>81</v>
@@ -1850,7 +1780,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B83">
         <v>82</v>
@@ -1861,7 +1791,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B84">
         <v>83</v>
@@ -1872,7 +1802,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B85">
         <v>84</v>
@@ -1883,7 +1813,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B86">
         <v>85</v>
@@ -1894,7 +1824,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B87">
         <v>86</v>
@@ -1905,7 +1835,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B88">
         <v>87</v>
@@ -1916,7 +1846,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B89">
         <v>88</v>
@@ -1927,7 +1857,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B90">
         <v>89</v>
@@ -1938,7 +1868,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B91">
         <v>90</v>
@@ -1949,7 +1879,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B92">
         <v>91</v>
@@ -1960,7 +1890,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B93">
         <v>92</v>
@@ -1971,7 +1901,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B94">
         <v>93</v>
@@ -1982,7 +1912,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B95">
         <v>94</v>
@@ -1993,7 +1923,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B96">
         <v>95</v>
@@ -2004,7 +1934,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B97">
         <v>96</v>
@@ -2015,7 +1945,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B98">
         <v>97</v>
@@ -2026,7 +1956,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B99">
         <v>98</v>
@@ -2037,7 +1967,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B100">
         <v>99</v>
@@ -2048,7 +1978,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B101">
         <v>100</v>
@@ -2059,7 +1989,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B102">
         <v>101</v>
@@ -2070,7 +2000,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B103">
         <v>102</v>
@@ -2081,7 +2011,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B104">
         <v>103</v>
@@ -2092,7 +2022,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B105">
         <v>104</v>
@@ -2103,7 +2033,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B106">
         <v>105</v>
@@ -2114,7 +2044,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B107">
         <v>106</v>
@@ -2125,7 +2055,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B108">
         <v>107</v>
@@ -2136,7 +2066,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B109">
         <v>108</v>
@@ -2147,7 +2077,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B110">
         <v>109</v>
@@ -2158,7 +2088,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B111">
         <v>110</v>
@@ -2169,7 +2099,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B112">
         <v>111</v>
@@ -2180,7 +2110,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B113">
         <v>112</v>
@@ -2191,7 +2121,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B114">
         <v>113</v>
@@ -2202,7 +2132,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B115">
         <v>114</v>
@@ -2213,7 +2143,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B116">
         <v>115</v>
@@ -2224,7 +2154,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B117">
         <v>116</v>
@@ -2235,7 +2165,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B118">
         <v>117</v>
@@ -2246,7 +2176,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B119">
         <v>118</v>
@@ -2257,7 +2187,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B120">
         <v>119</v>
@@ -2268,7 +2198,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B121">
         <v>120</v>
@@ -2279,7 +2209,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B122">
         <v>121</v>
@@ -2290,7 +2220,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B123">
         <v>122</v>
@@ -2301,7 +2231,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B124">
         <v>123</v>
@@ -2312,7 +2242,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B125">
         <v>124</v>
@@ -2323,7 +2253,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B126">
         <v>125</v>
@@ -2334,7 +2264,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B127">
         <v>126</v>
@@ -2345,7 +2275,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B128">
         <v>127</v>
@@ -2356,7 +2286,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B129">
         <v>128</v>
@@ -2367,7 +2297,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B130">
         <v>129</v>
@@ -2378,7 +2308,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B131">
         <v>130</v>
@@ -2389,7 +2319,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B132">
         <v>131</v>
@@ -2400,7 +2330,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B133">
         <v>132</v>
@@ -2411,7 +2341,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B134">
         <v>133</v>
@@ -2422,7 +2352,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B135">
         <v>134</v>
@@ -2433,7 +2363,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B136">
         <v>135</v>
@@ -2444,7 +2374,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B137">
         <v>136</v>
@@ -2455,7 +2385,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B138">
         <v>137</v>
@@ -2466,7 +2396,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B139">
         <v>138</v>
@@ -2477,7 +2407,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B140">
         <v>139</v>
@@ -2487,19 +2417,19 @@
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B141" s="3">
+      <c r="A141" t="s">
+        <v>147</v>
+      </c>
+      <c r="B141">
         <v>140</v>
       </c>
-      <c r="C141" s="3" t="s">
+      <c r="C141" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B142">
         <v>141</v>
@@ -2510,7 +2440,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B143">
         <v>142</v>
@@ -2521,7 +2451,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B144">
         <v>143</v>
@@ -2532,94 +2462,93 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B145">
         <v>144</v>
       </c>
       <c r="C145" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>152</v>
-      </c>
-      <c r="B146" t="s">
-        <v>152</v>
+        <v>153</v>
+      </c>
+      <c r="B146">
+        <v>145</v>
       </c>
       <c r="C146" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B147" s="2">
-        <v>145</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>154</v>
+      </c>
+      <c r="B147">
+        <v>146</v>
+      </c>
+      <c r="C147" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B148" s="5">
-        <v>146</v>
-      </c>
-      <c r="C148" s="5" t="s">
+      <c r="A148" t="s">
+        <v>155</v>
+      </c>
+      <c r="B148">
+        <v>147</v>
+      </c>
+      <c r="C148" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B149" s="5">
-        <v>147</v>
-      </c>
-      <c r="C149" s="5" t="s">
+      <c r="A149" t="s">
+        <v>156</v>
+      </c>
+      <c r="B149">
+        <v>148</v>
+      </c>
+      <c r="C149" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B150" s="5">
-        <v>148</v>
-      </c>
-      <c r="C150" s="5" t="s">
+      <c r="A150" t="s">
+        <v>157</v>
+      </c>
+      <c r="B150">
+        <v>149</v>
+      </c>
+      <c r="C150" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>157</v>
-      </c>
-      <c r="B151" s="5">
-        <v>149</v>
-      </c>
-      <c r="C151" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B151">
+        <v>150</v>
+      </c>
+      <c r="C151" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B152" s="5">
-        <v>150</v>
-      </c>
-      <c r="C152" s="5" t="s">
-        <v>7</v>
+      <c r="A152" t="s">
+        <v>159</v>
+      </c>
+      <c r="B152" t="s">
+        <v>159</v>
+      </c>
+      <c r="C152" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C151" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>